<commit_message>
use US data for indst/PPRiFUfICaWHR and indst/PPRiFUfIIaIoE
</commit_message>
<xml_diff>
--- a/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
+++ b/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\indst\PPRiFUfICaWHR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\indst\PPRiFUfICaWHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649E8F92-5031-4E5C-A383-AB9DE5FAA438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD78CF37-2349-42E0-A13A-10902176911B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="1620" windowWidth="23580" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="-17025" windowWidth="18390" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Source:</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>We do not apply this potential to non-manufacturing indutries due to their lack of large, heat-generating,</t>
+  </si>
+  <si>
+    <t>The EU EPS uses values from the US EPS.</t>
   </si>
 </sst>
 </file>
@@ -607,22 +610,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.1328125" customWidth="1"/>
+    <col min="3" max="3" width="29.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,39 +635,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2011</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -680,13 +690,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.59765625" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -694,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -702,7 +712,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -710,7 +720,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -719,7 +729,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -727,7 +737,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -750,13 +760,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47.86328125" customWidth="1"/>
+    <col min="2" max="2" width="23.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
@@ -764,7 +774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -772,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -780,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -788,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -796,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -805,7 +815,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -814,7 +824,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -823,7 +833,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -832,7 +842,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -841,7 +851,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -850,7 +860,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -859,7 +869,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -868,7 +878,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -877,7 +887,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -886,7 +896,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -895,7 +905,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -904,7 +914,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -913,7 +923,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -922,7 +932,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -931,7 +941,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -940,7 +950,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -949,7 +959,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -958,7 +968,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -966,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -974,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>39</v>
       </c>

</xml_diff>